<commit_message>
Various bug fixes and changes
</commit_message>
<xml_diff>
--- a/CDSImagingPilotProtocol_TimingsBlock1.xlsx
+++ b/CDSImagingPilotProtocol_TimingsBlock1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cchmc-my.sharepoint.com/personal/nicholas_dunn_cchmc_org/Documents/Documents/06 - Neuroimaging Study/SART/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research\Computerized Tasks\Sustained Attention to Response Task\sart-tp-psychopy-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_714DC67F0D7236ECF7985B67FD012D16618A1181" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{974866CA-56DF-493B-9275-6BDEDE0C7C31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443DF1B9-8C30-43D2-BA32-1F977C1CCA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="95">
   <si>
     <t>Non-target</t>
   </si>
@@ -278,54 +278,6 @@
     <t>Non-target</t>
   </si>
   <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
-    <t>Where was your attention focused?</t>
-  </si>
-  <si>
     <t>trialType</t>
   </si>
   <si>
@@ -363,6 +315,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Where was your attention focused just before the probe?</t>
   </si>
 </sst>
 </file>
@@ -412,10 +367,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -717,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,25 +683,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -770,7 +721,7 @@
         <v>1800</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -790,7 +741,7 @@
         <v>1800</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -810,7 +761,7 @@
         <v>1800</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -830,7 +781,7 @@
         <v>1800</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -850,7 +801,7 @@
         <v>1800</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -870,7 +821,7 @@
         <v>1800</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -890,7 +841,7 @@
         <v>1800</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -910,7 +861,7 @@
         <v>1800</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -930,7 +881,7 @@
         <v>1800</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -950,7 +901,7 @@
         <v>1800</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -970,7 +921,7 @@
         <v>1800</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -990,7 +941,7 @@
         <v>1800</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1010,7 +961,7 @@
         <v>1800</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1030,7 +981,7 @@
         <v>1800</v>
       </c>
       <c r="F15" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1050,7 +1001,7 @@
         <v>1800</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1070,7 +1021,7 @@
         <v>1800</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1090,7 +1041,7 @@
         <v>1800</v>
       </c>
       <c r="F18" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1110,7 +1061,7 @@
         <v>1800</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1130,7 +1081,7 @@
         <v>1800</v>
       </c>
       <c r="F20" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1150,7 +1101,7 @@
         <v>1800</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1170,7 +1121,7 @@
         <v>1800</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1190,7 +1141,7 @@
         <v>1800</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1210,7 +1161,7 @@
         <v>1800</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1230,7 +1181,7 @@
         <v>1800</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1250,7 +1201,7 @@
         <v>1800</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1270,7 +1221,7 @@
         <v>1800</v>
       </c>
       <c r="F27" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1290,7 +1241,7 @@
         <v>1800</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1310,7 +1261,7 @@
         <v>1800</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1330,7 +1281,7 @@
         <v>1800</v>
       </c>
       <c r="F30" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1350,7 +1301,7 @@
         <v>1800</v>
       </c>
       <c r="F31" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1370,7 +1321,7 @@
         <v>1800</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1390,7 +1341,7 @@
         <v>1800</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1410,7 +1361,7 @@
         <v>1800</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1430,7 +1381,7 @@
         <v>1800</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1450,7 +1401,7 @@
         <v>1800</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1470,7 +1421,7 @@
         <v>1800</v>
       </c>
       <c r="F37" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1490,7 +1441,7 @@
         <v>1800</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1510,7 +1461,7 @@
         <v>1800</v>
       </c>
       <c r="F39" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1530,7 +1481,7 @@
         <v>1800</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1550,7 +1501,7 @@
         <v>1800</v>
       </c>
       <c r="F41" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1570,7 +1521,7 @@
         <v>1800</v>
       </c>
       <c r="F42" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1590,7 +1541,7 @@
         <v>1800</v>
       </c>
       <c r="F43" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1610,7 +1561,7 @@
         <v>1800</v>
       </c>
       <c r="F44" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1630,7 +1581,7 @@
         <v>1800</v>
       </c>
       <c r="F45" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1650,7 +1601,7 @@
         <v>1800</v>
       </c>
       <c r="F46" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1670,7 +1621,7 @@
         <v>1800</v>
       </c>
       <c r="F47" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1690,7 +1641,7 @@
         <v>1800</v>
       </c>
       <c r="F48" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1710,7 +1661,7 @@
         <v>1800</v>
       </c>
       <c r="F49" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1730,7 +1681,7 @@
         <v>1800</v>
       </c>
       <c r="F50" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1750,7 +1701,7 @@
         <v>1800</v>
       </c>
       <c r="F51" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1770,7 +1721,7 @@
         <v>1800</v>
       </c>
       <c r="F52" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1790,7 +1741,7 @@
         <v>1800</v>
       </c>
       <c r="F53" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1810,7 +1761,7 @@
         <v>1800</v>
       </c>
       <c r="F54" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1830,7 +1781,7 @@
         <v>1800</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1850,7 +1801,7 @@
         <v>1800</v>
       </c>
       <c r="F56" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1870,7 +1821,7 @@
         <v>1800</v>
       </c>
       <c r="F57" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1890,7 +1841,7 @@
         <v>1800</v>
       </c>
       <c r="F58" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1898,7 +1849,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C59">
         <v>142500</v>
@@ -1915,7 +1866,7 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C60">
         <v>148500</v>
@@ -1927,7 +1878,7 @@
         <v>5000</v>
       </c>
       <c r="G60" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1947,7 +1898,7 @@
         <v>1800</v>
       </c>
       <c r="F61" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1967,7 +1918,7 @@
         <v>1800</v>
       </c>
       <c r="F62" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1987,7 +1938,7 @@
         <v>1800</v>
       </c>
       <c r="F63" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2007,7 +1958,7 @@
         <v>1800</v>
       </c>
       <c r="F64" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2027,7 +1978,7 @@
         <v>1800</v>
       </c>
       <c r="F65" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2047,7 +1998,7 @@
         <v>1800</v>
       </c>
       <c r="F66" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2067,7 +2018,7 @@
         <v>1800</v>
       </c>
       <c r="F67" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2087,7 +2038,7 @@
         <v>1800</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2107,7 +2058,7 @@
         <v>1800</v>
       </c>
       <c r="F69" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2127,7 +2078,7 @@
         <v>1800</v>
       </c>
       <c r="F70" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2147,7 +2098,7 @@
         <v>1800</v>
       </c>
       <c r="F71" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2167,7 +2118,7 @@
         <v>1800</v>
       </c>
       <c r="F72" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2175,7 +2126,7 @@
         <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C73">
         <v>184500</v>
@@ -2187,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2195,7 +2146,7 @@
         <v>15</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C74">
         <v>190500</v>
@@ -2207,7 +2158,7 @@
         <v>5000</v>
       </c>
       <c r="G74" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2227,7 +2178,7 @@
         <v>1800</v>
       </c>
       <c r="F75" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2247,7 +2198,7 @@
         <v>1800</v>
       </c>
       <c r="F76" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2267,7 +2218,7 @@
         <v>1800</v>
       </c>
       <c r="F77" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2287,7 +2238,7 @@
         <v>1800</v>
       </c>
       <c r="F78" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2307,7 +2258,7 @@
         <v>1800</v>
       </c>
       <c r="F79" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2327,7 +2278,7 @@
         <v>1800</v>
       </c>
       <c r="F80" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2347,7 +2298,7 @@
         <v>1800</v>
       </c>
       <c r="F81" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2367,7 +2318,7 @@
         <v>1800</v>
       </c>
       <c r="F82" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2387,7 +2338,7 @@
         <v>1800</v>
       </c>
       <c r="F83" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2407,7 +2358,7 @@
         <v>1800</v>
       </c>
       <c r="F84" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2427,7 +2378,7 @@
         <v>1800</v>
       </c>
       <c r="F85" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2447,7 +2398,7 @@
         <v>1800</v>
       </c>
       <c r="F86" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2467,7 +2418,7 @@
         <v>1800</v>
       </c>
       <c r="F87" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2487,7 +2438,7 @@
         <v>1800</v>
       </c>
       <c r="F88" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2507,7 +2458,7 @@
         <v>1800</v>
       </c>
       <c r="F89" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2527,7 +2478,7 @@
         <v>1800</v>
       </c>
       <c r="F90" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2547,7 +2498,7 @@
         <v>1800</v>
       </c>
       <c r="F91" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2555,7 +2506,7 @@
         <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C92">
         <v>239000</v>
@@ -2567,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2575,7 +2526,7 @@
         <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C93">
         <v>245000</v>
@@ -2587,7 +2538,7 @@
         <v>5000</v>
       </c>
       <c r="G93" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2607,7 +2558,7 @@
         <v>1800</v>
       </c>
       <c r="F94" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2627,7 +2578,7 @@
         <v>1800</v>
       </c>
       <c r="F95" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2647,7 +2598,7 @@
         <v>1800</v>
       </c>
       <c r="F96" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2667,7 +2618,7 @@
         <v>1800</v>
       </c>
       <c r="F97" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2687,7 +2638,7 @@
         <v>1800</v>
       </c>
       <c r="F98" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2707,7 +2658,7 @@
         <v>1800</v>
       </c>
       <c r="F99" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2727,7 +2678,7 @@
         <v>1800</v>
       </c>
       <c r="F100" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2747,7 +2698,7 @@
         <v>1800</v>
       </c>
       <c r="F101" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2767,7 +2718,7 @@
         <v>1800</v>
       </c>
       <c r="F102" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2787,7 +2738,7 @@
         <v>1800</v>
       </c>
       <c r="F103" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2807,7 +2758,7 @@
         <v>1800</v>
       </c>
       <c r="F104" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2827,7 +2778,7 @@
         <v>1800</v>
       </c>
       <c r="F105" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2847,7 +2798,7 @@
         <v>1800</v>
       </c>
       <c r="F106" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2855,7 +2806,7 @@
         <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C107">
         <v>283500</v>
@@ -2867,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2875,7 +2826,7 @@
         <v>23</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C108">
         <v>289500</v>
@@ -2887,7 +2838,7 @@
         <v>5000</v>
       </c>
       <c r="G108" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2907,7 +2858,7 @@
         <v>1800</v>
       </c>
       <c r="F109" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2927,7 +2878,7 @@
         <v>1800</v>
       </c>
       <c r="F110" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2947,7 +2898,7 @@
         <v>1800</v>
       </c>
       <c r="F111" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2967,7 +2918,7 @@
         <v>1800</v>
       </c>
       <c r="F112" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2987,7 +2938,7 @@
         <v>1800</v>
       </c>
       <c r="F113" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3007,7 +2958,7 @@
         <v>1800</v>
       </c>
       <c r="F114" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3015,7 +2966,7 @@
         <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C115">
         <v>310500</v>
@@ -3027,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3035,7 +2986,7 @@
         <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C116">
         <v>316500</v>
@@ -3047,7 +2998,7 @@
         <v>5000</v>
       </c>
       <c r="G116" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3067,7 +3018,7 @@
         <v>1800</v>
       </c>
       <c r="F117" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3087,7 +3038,7 @@
         <v>1800</v>
       </c>
       <c r="F118" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3107,7 +3058,7 @@
         <v>1800</v>
       </c>
       <c r="F119" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3127,7 +3078,7 @@
         <v>1800</v>
       </c>
       <c r="F120" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3147,7 +3098,7 @@
         <v>1800</v>
       </c>
       <c r="F121" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3167,7 +3118,7 @@
         <v>1800</v>
       </c>
       <c r="F122" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3187,7 +3138,7 @@
         <v>1800</v>
       </c>
       <c r="F123" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3207,7 +3158,7 @@
         <v>1800</v>
       </c>
       <c r="F124" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3227,7 +3178,7 @@
         <v>1800</v>
       </c>
       <c r="F125" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3247,7 +3198,7 @@
         <v>1800</v>
       </c>
       <c r="F126" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3267,7 +3218,7 @@
         <v>1800</v>
       </c>
       <c r="F127" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3287,7 +3238,7 @@
         <v>1800</v>
       </c>
       <c r="F128" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3307,7 +3258,7 @@
         <v>1800</v>
       </c>
       <c r="F129" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3327,7 +3278,7 @@
         <v>1800</v>
       </c>
       <c r="F130" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3347,7 +3298,7 @@
         <v>1800</v>
       </c>
       <c r="F131" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3367,7 +3318,7 @@
         <v>1800</v>
       </c>
       <c r="F132" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3387,7 +3338,7 @@
         <v>1800</v>
       </c>
       <c r="F133" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3407,7 +3358,7 @@
         <v>1800</v>
       </c>
       <c r="F134" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3427,7 +3378,7 @@
         <v>1800</v>
       </c>
       <c r="F135" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3447,7 +3398,7 @@
         <v>1800</v>
       </c>
       <c r="F136" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3455,7 +3406,7 @@
         <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C137">
         <v>372500</v>
@@ -3467,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="F137" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3475,7 +3426,7 @@
         <v>31</v>
       </c>
       <c r="B138" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C138">
         <v>378500</v>
@@ -3487,7 +3438,7 @@
         <v>5000</v>
       </c>
       <c r="G138" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3507,7 +3458,7 @@
         <v>1800</v>
       </c>
       <c r="F139" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3527,7 +3478,7 @@
         <v>1800</v>
       </c>
       <c r="F140" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3547,7 +3498,7 @@
         <v>1800</v>
       </c>
       <c r="F141" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3567,7 +3518,7 @@
         <v>1800</v>
       </c>
       <c r="F142" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3587,7 +3538,7 @@
         <v>1800</v>
       </c>
       <c r="F143" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3607,7 +3558,7 @@
         <v>1800</v>
       </c>
       <c r="F144" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3627,7 +3578,7 @@
         <v>1800</v>
       </c>
       <c r="F145" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3635,7 +3586,7 @@
         <v>33</v>
       </c>
       <c r="B146" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C146">
         <v>402000</v>
@@ -3647,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="F146" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3655,7 +3606,7 @@
         <v>34</v>
       </c>
       <c r="B147" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C147">
         <v>408000</v>
@@ -3667,7 +3618,7 @@
         <v>5000</v>
       </c>
       <c r="G147" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3687,7 +3638,7 @@
         <v>1800</v>
       </c>
       <c r="F148" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3707,7 +3658,7 @@
         <v>1800</v>
       </c>
       <c r="F149" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3727,7 +3678,7 @@
         <v>1800</v>
       </c>
       <c r="F150" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3747,7 +3698,7 @@
         <v>1800</v>
       </c>
       <c r="F151" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3767,7 +3718,7 @@
         <v>1800</v>
       </c>
       <c r="F152" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3787,7 +3738,7 @@
         <v>1800</v>
       </c>
       <c r="F153" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3807,7 +3758,7 @@
         <v>1800</v>
       </c>
       <c r="F154" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3827,7 +3778,7 @@
         <v>1800</v>
       </c>
       <c r="F155" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3847,7 +3798,7 @@
         <v>1800</v>
       </c>
       <c r="F156" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -3867,7 +3818,7 @@
         <v>1800</v>
       </c>
       <c r="F157" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -3887,7 +3838,7 @@
         <v>1800</v>
       </c>
       <c r="F158" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -3907,7 +3858,7 @@
         <v>1800</v>
       </c>
       <c r="F159" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -3927,7 +3878,7 @@
         <v>1800</v>
       </c>
       <c r="F160" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -3947,7 +3898,7 @@
         <v>1800</v>
       </c>
       <c r="F161" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -3967,7 +3918,7 @@
         <v>1800</v>
       </c>
       <c r="F162" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -3987,7 +3938,7 @@
         <v>1800</v>
       </c>
       <c r="F163" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4007,7 +3958,7 @@
         <v>1800</v>
       </c>
       <c r="F164" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4027,7 +3978,7 @@
         <v>1800</v>
       </c>
       <c r="F165" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4047,7 +3998,7 @@
         <v>1800</v>
       </c>
       <c r="F166" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -4067,7 +4018,7 @@
         <v>1800</v>
       </c>
       <c r="F167" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4087,7 +4038,7 @@
         <v>1800</v>
       </c>
       <c r="F168" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4095,7 +4046,7 @@
         <v>38</v>
       </c>
       <c r="B169" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C169">
         <v>466500</v>
@@ -4107,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="F169" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4115,7 +4066,7 @@
         <v>39</v>
       </c>
       <c r="B170" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C170">
         <v>472500</v>
@@ -4127,7 +4078,7 @@
         <v>5000</v>
       </c>
       <c r="G170" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4147,7 +4098,7 @@
         <v>1800</v>
       </c>
       <c r="F171" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4167,7 +4118,7 @@
         <v>1800</v>
       </c>
       <c r="F172" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4187,7 +4138,7 @@
         <v>1800</v>
       </c>
       <c r="F173" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4207,7 +4158,7 @@
         <v>1800</v>
       </c>
       <c r="F174" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4227,7 +4178,7 @@
         <v>1800</v>
       </c>
       <c r="F175" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4247,7 +4198,7 @@
         <v>1800</v>
       </c>
       <c r="F176" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4267,7 +4218,7 @@
         <v>1800</v>
       </c>
       <c r="F177" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4287,7 +4238,7 @@
         <v>1800</v>
       </c>
       <c r="F178" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4307,7 +4258,7 @@
         <v>1800</v>
       </c>
       <c r="F179" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4327,7 +4278,7 @@
         <v>1800</v>
       </c>
       <c r="F180" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4347,7 +4298,7 @@
         <v>1800</v>
       </c>
       <c r="F181" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4355,7 +4306,7 @@
         <v>41</v>
       </c>
       <c r="B182" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C182">
         <v>506000</v>
@@ -4367,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="F182" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4375,7 +4326,7 @@
         <v>42</v>
       </c>
       <c r="B183" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C183">
         <v>512000</v>
@@ -4387,7 +4338,7 @@
         <v>5000</v>
       </c>
       <c r="G183" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4407,7 +4358,7 @@
         <v>1800</v>
       </c>
       <c r="F184" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4427,7 +4378,7 @@
         <v>1800</v>
       </c>
       <c r="F185" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -4447,7 +4398,7 @@
         <v>1800</v>
       </c>
       <c r="F186" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -4467,7 +4418,7 @@
         <v>1800</v>
       </c>
       <c r="F187" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -4487,7 +4438,7 @@
         <v>1800</v>
       </c>
       <c r="F188" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -4507,7 +4458,7 @@
         <v>1800</v>
       </c>
       <c r="F189" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -4527,7 +4478,7 @@
         <v>1800</v>
       </c>
       <c r="F190" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -4547,7 +4498,7 @@
         <v>1800</v>
       </c>
       <c r="F191" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4567,7 +4518,7 @@
         <v>1800</v>
       </c>
       <c r="F192" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4587,7 +4538,7 @@
         <v>1800</v>
       </c>
       <c r="F193" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4607,7 +4558,7 @@
         <v>1800</v>
       </c>
       <c r="F194" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4627,7 +4578,7 @@
         <v>1800</v>
       </c>
       <c r="F195" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4647,7 +4598,7 @@
         <v>1800</v>
       </c>
       <c r="F196" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4667,7 +4618,7 @@
         <v>1800</v>
       </c>
       <c r="F197" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4675,7 +4626,7 @@
         <v>46</v>
       </c>
       <c r="B198" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C198">
         <v>553000</v>
@@ -4687,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="F198" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4695,7 +4646,7 @@
         <v>47</v>
       </c>
       <c r="B199" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C199">
         <v>559000</v>
@@ -4707,7 +4658,7 @@
         <v>5000</v>
       </c>
       <c r="G199" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4727,7 +4678,7 @@
         <v>1800</v>
       </c>
       <c r="F200" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -4747,7 +4698,7 @@
         <v>1800</v>
       </c>
       <c r="F201" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -4767,7 +4718,7 @@
         <v>1800</v>
       </c>
       <c r="F202" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -4787,7 +4738,7 @@
         <v>1800</v>
       </c>
       <c r="F203" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -4807,7 +4758,7 @@
         <v>1800</v>
       </c>
       <c r="F204" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -4827,7 +4778,7 @@
         <v>1800</v>
       </c>
       <c r="F205" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -4847,7 +4798,7 @@
         <v>1800</v>
       </c>
       <c r="F206" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -4867,7 +4818,7 @@
         <v>1800</v>
       </c>
       <c r="F207" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -4887,7 +4838,7 @@
         <v>1800</v>
       </c>
       <c r="F208" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -4907,7 +4858,7 @@
         <v>1800</v>
       </c>
       <c r="F209" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -4927,7 +4878,7 @@
         <v>1800</v>
       </c>
       <c r="F210" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -4947,7 +4898,7 @@
         <v>1800</v>
       </c>
       <c r="F211" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -4967,7 +4918,7 @@
         <v>1800</v>
       </c>
       <c r="F212" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -4987,7 +4938,7 @@
         <v>1800</v>
       </c>
       <c r="F213" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -5007,7 +4958,7 @@
         <v>1800</v>
       </c>
       <c r="F214" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -5027,7 +4978,7 @@
         <v>1800</v>
       </c>
       <c r="F215" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5047,7 +4998,7 @@
         <v>1800</v>
       </c>
       <c r="F216" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -5067,7 +5018,7 @@
         <v>1800</v>
       </c>
       <c r="F217" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -5087,7 +5038,7 @@
         <v>1800</v>
       </c>
       <c r="F218" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -5107,7 +5058,7 @@
         <v>1800</v>
       </c>
       <c r="F219" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -5127,7 +5078,7 @@
         <v>1800</v>
       </c>
       <c r="F220" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5147,7 +5098,7 @@
         <v>1800</v>
       </c>
       <c r="F221" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -5167,7 +5118,7 @@
         <v>1800</v>
       </c>
       <c r="F222" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -5187,7 +5138,7 @@
         <v>1800</v>
       </c>
       <c r="F223" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -5207,7 +5158,7 @@
         <v>1800</v>
       </c>
       <c r="F224" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -5227,7 +5178,7 @@
         <v>1800</v>
       </c>
       <c r="F225" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -5247,7 +5198,7 @@
         <v>1800</v>
       </c>
       <c r="F226" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -5267,7 +5218,7 @@
         <v>1800</v>
       </c>
       <c r="F227" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -5287,7 +5238,7 @@
         <v>1800</v>
       </c>
       <c r="F228" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -5307,7 +5258,7 @@
         <v>1800</v>
       </c>
       <c r="F229" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -5327,7 +5278,7 @@
         <v>1800</v>
       </c>
       <c r="F230" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -5347,7 +5298,7 @@
         <v>1800</v>
       </c>
       <c r="F231" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -5367,7 +5318,7 @@
         <v>1800</v>
       </c>
       <c r="F232" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -5387,7 +5338,7 @@
         <v>1800</v>
       </c>
       <c r="F233" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -5407,7 +5358,7 @@
         <v>1800</v>
       </c>
       <c r="F234" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -5427,7 +5378,7 @@
         <v>1800</v>
       </c>
       <c r="F235" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -5447,7 +5398,7 @@
         <v>1800</v>
       </c>
       <c r="F236" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -5467,7 +5418,7 @@
         <v>1800</v>
       </c>
       <c r="F237" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -5487,7 +5438,7 @@
         <v>1800</v>
       </c>
       <c r="F238" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -5507,7 +5458,7 @@
         <v>1800</v>
       </c>
       <c r="F239" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -5527,7 +5478,7 @@
         <v>1800</v>
       </c>
       <c r="F240" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5547,7 +5498,7 @@
         <v>1800</v>
       </c>
       <c r="F241" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5567,7 +5518,7 @@
         <v>1800</v>
       </c>
       <c r="F242" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5587,7 +5538,7 @@
         <v>1800</v>
       </c>
       <c r="F243" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -5607,7 +5558,7 @@
         <v>1800</v>
       </c>
       <c r="F244" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -5615,7 +5566,7 @@
         <v>55</v>
       </c>
       <c r="B245" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C245">
         <v>677500</v>
@@ -5627,7 +5578,7 @@
         <v>0</v>
       </c>
       <c r="F245" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -5635,7 +5586,7 @@
         <v>56</v>
       </c>
       <c r="B246" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C246">
         <v>683500</v>
@@ -5647,7 +5598,7 @@
         <v>5000</v>
       </c>
       <c r="G246" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -5667,7 +5618,7 @@
         <v>1800</v>
       </c>
       <c r="F247" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -5687,7 +5638,7 @@
         <v>1800</v>
       </c>
       <c r="F248" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -5707,7 +5658,7 @@
         <v>1800</v>
       </c>
       <c r="F249" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -5727,7 +5678,7 @@
         <v>1800</v>
       </c>
       <c r="F250" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -5747,7 +5698,7 @@
         <v>1800</v>
       </c>
       <c r="F251" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -5755,7 +5706,7 @@
         <v>58</v>
       </c>
       <c r="B252" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C252">
         <v>702000</v>
@@ -5767,7 +5718,7 @@
         <v>0</v>
       </c>
       <c r="F252" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -5775,7 +5726,7 @@
         <v>59</v>
       </c>
       <c r="B253" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C253">
         <v>708000</v>
@@ -5787,7 +5738,7 @@
         <v>5000</v>
       </c>
       <c r="G253" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -5807,7 +5758,7 @@
         <v>1800</v>
       </c>
       <c r="F254" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -5827,7 +5778,7 @@
         <v>1800</v>
       </c>
       <c r="F255" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -5847,7 +5798,7 @@
         <v>1800</v>
       </c>
       <c r="F256" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -5867,7 +5818,7 @@
         <v>1800</v>
       </c>
       <c r="F257" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -5887,7 +5838,7 @@
         <v>1800</v>
       </c>
       <c r="F258" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -5907,7 +5858,7 @@
         <v>1800</v>
       </c>
       <c r="F259" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -5927,7 +5878,7 @@
         <v>1800</v>
       </c>
       <c r="F260" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -5947,7 +5898,7 @@
         <v>1800</v>
       </c>
       <c r="F261" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -5967,7 +5918,7 @@
         <v>1800</v>
       </c>
       <c r="F262" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -5987,7 +5938,7 @@
         <v>1800</v>
       </c>
       <c r="F263" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6007,7 +5958,7 @@
         <v>1800</v>
       </c>
       <c r="F264" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6027,7 +5978,7 @@
         <v>1800</v>
       </c>
       <c r="F265" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6035,7 +5986,7 @@
         <v>61</v>
       </c>
       <c r="B266" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C266">
         <v>744000</v>
@@ -6047,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="F266" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6055,7 +6006,7 @@
         <v>62</v>
       </c>
       <c r="B267" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C267">
         <v>750000</v>
@@ -6067,7 +6018,7 @@
         <v>5000</v>
       </c>
       <c r="G267" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6087,7 +6038,7 @@
         <v>1800</v>
       </c>
       <c r="F268" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6107,7 +6058,7 @@
         <v>1800</v>
       </c>
       <c r="F269" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6127,7 +6078,7 @@
         <v>1800</v>
       </c>
       <c r="F270" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6147,7 +6098,7 @@
         <v>1800</v>
       </c>
       <c r="F271" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6167,7 +6118,7 @@
         <v>1800</v>
       </c>
       <c r="F272" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6187,7 +6138,7 @@
         <v>0</v>
       </c>
       <c r="F273" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6195,7 +6146,7 @@
         <v>65</v>
       </c>
       <c r="B274" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C274">
         <v>774500</v>
@@ -6207,7 +6158,7 @@
         <v>5000</v>
       </c>
       <c r="G274" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6227,7 +6178,7 @@
         <v>1800</v>
       </c>
       <c r="F275" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6247,7 +6198,7 @@
         <v>1800</v>
       </c>
       <c r="F276" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6267,7 +6218,7 @@
         <v>1800</v>
       </c>
       <c r="F277" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6287,7 +6238,7 @@
         <v>1800</v>
       </c>
       <c r="F278" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6307,7 +6258,7 @@
         <v>1800</v>
       </c>
       <c r="F279" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6327,7 +6278,7 @@
         <v>1800</v>
       </c>
       <c r="F280" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6347,7 +6298,7 @@
         <v>1800</v>
       </c>
       <c r="F281" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6367,7 +6318,7 @@
         <v>1800</v>
       </c>
       <c r="F282" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6387,7 +6338,7 @@
         <v>1800</v>
       </c>
       <c r="F283" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6407,7 +6358,7 @@
         <v>1800</v>
       </c>
       <c r="F284" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6427,7 +6378,7 @@
         <v>1800</v>
       </c>
       <c r="F285" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6447,7 +6398,7 @@
         <v>1800</v>
       </c>
       <c r="F286" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6467,7 +6418,7 @@
         <v>1800</v>
       </c>
       <c r="F287" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -6487,7 +6438,7 @@
         <v>1800</v>
       </c>
       <c r="F288" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="289" spans="1:6">
@@ -6507,7 +6458,7 @@
         <v>1800</v>
       </c>
       <c r="F289" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="290" spans="1:6">
@@ -6527,7 +6478,7 @@
         <v>1800</v>
       </c>
       <c r="F290" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="291" spans="1:6">
@@ -6547,7 +6498,7 @@
         <v>1800</v>
       </c>
       <c r="F291" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="292" spans="1:6">
@@ -6567,7 +6518,7 @@
         <v>1800</v>
       </c>
       <c r="F292" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="293" spans="1:6">
@@ -6587,7 +6538,7 @@
         <v>1800</v>
       </c>
       <c r="F293" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="294" spans="1:6">
@@ -6607,7 +6558,7 @@
         <v>1800</v>
       </c>
       <c r="F294" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="295" spans="1:6">
@@ -6627,7 +6578,7 @@
         <v>1800</v>
       </c>
       <c r="F295" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="296" spans="1:6">
@@ -6647,7 +6598,7 @@
         <v>1800</v>
       </c>
       <c r="F296" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="297" spans="1:6">
@@ -6667,7 +6618,7 @@
         <v>1800</v>
       </c>
       <c r="F297" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="298" spans="1:6">
@@ -6687,7 +6638,7 @@
         <v>1800</v>
       </c>
       <c r="F298" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="299" spans="1:6">
@@ -6707,7 +6658,7 @@
         <v>1800</v>
       </c>
       <c r="F299" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="300" spans="1:6">
@@ -6727,7 +6678,7 @@
         <v>1800</v>
       </c>
       <c r="F300" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="301" spans="1:6">
@@ -6747,7 +6698,7 @@
         <v>1800</v>
       </c>
       <c r="F301" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="302" spans="1:6">
@@ -6767,7 +6718,7 @@
         <v>1800</v>
       </c>
       <c r="F302" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="303" spans="1:6">
@@ -6787,7 +6738,7 @@
         <v>1800</v>
       </c>
       <c r="F303" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="304" spans="1:6">
@@ -6795,7 +6746,7 @@
         <v>69</v>
       </c>
       <c r="B304" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C304">
         <v>853000</v>
@@ -6807,7 +6758,7 @@
         <v>0</v>
       </c>
       <c r="F304" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -6815,7 +6766,7 @@
         <v>70</v>
       </c>
       <c r="B305" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C305">
         <v>859000</v>
@@ -6827,7 +6778,7 @@
         <v>5000</v>
       </c>
       <c r="G305" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -6847,7 +6798,7 @@
         <v>1800</v>
       </c>
       <c r="F306" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -6867,7 +6818,7 @@
         <v>1800</v>
       </c>
       <c r="F307" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -6887,7 +6838,7 @@
         <v>1800</v>
       </c>
       <c r="F308" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -6907,7 +6858,7 @@
         <v>1800</v>
       </c>
       <c r="F309" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -6927,7 +6878,7 @@
         <v>1800</v>
       </c>
       <c r="F310" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -6947,7 +6898,7 @@
         <v>1800</v>
       </c>
       <c r="F311" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -6967,7 +6918,7 @@
         <v>1800</v>
       </c>
       <c r="F312" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -6987,7 +6938,7 @@
         <v>1800</v>
       </c>
       <c r="F313" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -7007,7 +6958,7 @@
         <v>1800</v>
       </c>
       <c r="F314" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -7027,7 +6978,7 @@
         <v>1800</v>
       </c>
       <c r="F315" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -7035,7 +6986,7 @@
         <v>72</v>
       </c>
       <c r="B316" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C316">
         <v>890000</v>
@@ -7047,7 +6998,7 @@
         <v>0</v>
       </c>
       <c r="F316" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -7055,7 +7006,7 @@
         <v>73</v>
       </c>
       <c r="B317" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C317">
         <v>896000</v>
@@ -7067,7 +7018,7 @@
         <v>5000</v>
       </c>
       <c r="G317" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -7087,7 +7038,7 @@
         <v>1800</v>
       </c>
       <c r="F318" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7107,7 +7058,7 @@
         <v>1800</v>
       </c>
       <c r="F319" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7127,7 +7078,7 @@
         <v>1800</v>
       </c>
       <c r="F320" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -7147,7 +7098,7 @@
         <v>1800</v>
       </c>
       <c r="F321" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="322" spans="1:6">
@@ -7167,7 +7118,7 @@
         <v>1800</v>
       </c>
       <c r="F322" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="323" spans="1:6">
@@ -7187,7 +7138,7 @@
         <v>1800</v>
       </c>
       <c r="F323" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -7207,7 +7158,7 @@
         <v>1800</v>
       </c>
       <c r="F324" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="325" spans="1:6">
@@ -7227,7 +7178,7 @@
         <v>1800</v>
       </c>
       <c r="F325" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -7247,7 +7198,7 @@
         <v>1800</v>
       </c>
       <c r="F326" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="327" spans="1:6">
@@ -7267,7 +7218,7 @@
         <v>1800</v>
       </c>
       <c r="F327" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="328" spans="1:6">
@@ -7287,7 +7238,7 @@
         <v>1800</v>
       </c>
       <c r="F328" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="329" spans="1:6">
@@ -7307,7 +7258,7 @@
         <v>1800</v>
       </c>
       <c r="F329" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="330" spans="1:6">
@@ -7327,7 +7278,7 @@
         <v>1800</v>
       </c>
       <c r="F330" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="331" spans="1:6">
@@ -7347,7 +7298,7 @@
         <v>1800</v>
       </c>
       <c r="F331" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="332" spans="1:6">
@@ -7367,7 +7318,7 @@
         <v>1800</v>
       </c>
       <c r="F332" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="333" spans="1:6">
@@ -7387,7 +7338,7 @@
         <v>1800</v>
       </c>
       <c r="F333" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="334" spans="1:6">
@@ -7407,7 +7358,7 @@
         <v>1800</v>
       </c>
       <c r="F334" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="335" spans="1:6">
@@ -7427,7 +7378,7 @@
         <v>1800</v>
       </c>
       <c r="F335" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="336" spans="1:6">
@@ -7447,7 +7398,7 @@
         <v>1800</v>
       </c>
       <c r="F336" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="337" spans="1:6">
@@ -7467,7 +7418,7 @@
         <v>1800</v>
       </c>
       <c r="F337" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="338" spans="1:6">
@@ -7487,7 +7438,7 @@
         <v>1800</v>
       </c>
       <c r="F338" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="339" spans="1:6">
@@ -7507,7 +7458,7 @@
         <v>1800</v>
       </c>
       <c r="F339" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="340" spans="1:6">
@@ -7527,7 +7478,7 @@
         <v>1800</v>
       </c>
       <c r="F340" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="341" spans="1:6">
@@ -7547,7 +7498,7 @@
         <v>1800</v>
       </c>
       <c r="F341" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="342" spans="1:6">
@@ -7567,7 +7518,7 @@
         <v>1800</v>
       </c>
       <c r="F342" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="343" spans="1:6">
@@ -7587,7 +7538,7 @@
         <v>1800</v>
       </c>
       <c r="F343" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -7607,7 +7558,7 @@
         <v>1800</v>
       </c>
       <c r="F344" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -7627,7 +7578,7 @@
         <v>1800</v>
       </c>
       <c r="F345" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -7647,7 +7598,7 @@
         <v>1800</v>
       </c>
       <c r="F346" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>